<commit_message>
Finish this completely useless exercise in trying to reorder this script, and then realizing that was a terrible idea
</commit_message>
<xml_diff>
--- a/data/raw/01b_edited-species8_location-independent-final-fix.xlsx
+++ b/data/raw/01b_edited-species8_location-independent-final-fix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:40009_{8A6DA30E-687F-47E7-A24D-C265325037DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65C656CF-0C0C-4C9C-9033-456660A43C83}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:40009_{8A6DA30E-687F-47E7-A24D-C265325037DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E51E6AA-B9BF-4070-9942-A9A3913372E1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,89 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={65E51169-7DDF-431B-97D7-5AC86993A7BF}</author>
+    <author>tc={24D482F9-3F79-4447-838B-FD4C665F3D67}</author>
+    <author>tc={BF13A08C-3A83-4A87-89AA-5677AE747C03}</author>
+    <author>tc={C221EFA2-F912-4135-981C-E7AF98A329A9}</author>
+    <author>tc={2F5931CB-DF6B-4F53-9005-53E77F3E2987}</author>
+    <author>tc={C6172F8C-64D1-435B-B6C6-C054FCF63812}</author>
+    <author>tc={7A5A69C5-6672-4327-A71A-D60D0159BC65}</author>
+    <author>tc={5B1E393E-188A-4FCD-87DD-803EDEB5A732}</author>
+  </authors>
+  <commentList>
+    <comment ref="B194" authorId="0" shapeId="0" xr:uid="{65E51169-7DDF-431B-97D7-5AC86993A7BF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Originally was "ELEL6", which was likely a mistake from dragging and copying the cell above at some point.</t>
+      </text>
+    </comment>
+    <comment ref="B195" authorId="1" shapeId="0" xr:uid="{24D482F9-3F79-4447-838B-FD4C665F3D67}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Originally was "ELEL7", which was likely a mistake from dragging and copying the cell above at some point.</t>
+      </text>
+    </comment>
+    <comment ref="B224" authorId="2" shapeId="0" xr:uid="{BF13A08C-3A83-4A87-89AA-5677AE747C03}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is the official USDA Plants code</t>
+      </text>
+    </comment>
+    <comment ref="B225" authorId="3" shapeId="0" xr:uid="{C221EFA2-F912-4135-981C-E7AF98A329A9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is the official USDA Plants code</t>
+      </text>
+    </comment>
+    <comment ref="B372" authorId="4" shapeId="0" xr:uid="{2F5931CB-DF6B-4F53-9005-53E77F3E2987}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Originally was "SPAM3", which was likely a mistake from dragging and copying the cell above at some point.</t>
+      </text>
+    </comment>
+    <comment ref="B373" authorId="5" shapeId="0" xr:uid="{C6172F8C-64D1-435B-B6C6-C054FCF63812}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Originally was "SPAM4", which was likely a mistake from dragging and copying the cell above at some point.</t>
+      </text>
+    </comment>
+    <comment ref="B374" authorId="6" shapeId="0" xr:uid="{7A5A69C5-6672-4327-A71A-D60D0159BC65}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Originally was "SPAM5", which was likely a mistake from dragging and copying the cell above at some point.</t>
+      </text>
+    </comment>
+    <comment ref="B391" authorId="7" shapeId="0" xr:uid="{5B1E393E-188A-4FCD-87DD-803EDEB5A732}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is the official USDA Plants code</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2356" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2356" uniqueCount="601">
   <si>
     <t>CodeOriginal</t>
   </si>
@@ -1814,13 +1895,22 @@
   </si>
   <si>
     <t>Zinnia grandiflora</t>
+  </si>
+  <si>
+    <t>CHAB2</t>
+  </si>
+  <si>
+    <t>CHME5</t>
+  </si>
+  <si>
+    <t>MILI5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1960,6 +2050,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="34">
@@ -2445,6 +2541,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Ossanna, Lia Qin Ryan - (lossanna)" id="{F2C253AE-3829-426F-8607-10F478AAC97A}" userId="S::lossanna@arizona.edu::4ef914cd-790d-460d-a4af-cca4fc5cf0d2" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2740,13 +2842,42 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B194" dT="2023-09-11T22:12:56.03" personId="{F2C253AE-3829-426F-8607-10F478AAC97A}" id="{65E51169-7DDF-431B-97D7-5AC86993A7BF}">
+    <text>Originally was "ELEL6", which was likely a mistake from dragging and copying the cell above at some point.</text>
+  </threadedComment>
+  <threadedComment ref="B195" dT="2023-09-11T22:13:06.21" personId="{F2C253AE-3829-426F-8607-10F478AAC97A}" id="{24D482F9-3F79-4447-838B-FD4C665F3D67}">
+    <text>Originally was "ELEL7", which was likely a mistake from dragging and copying the cell above at some point.</text>
+  </threadedComment>
+  <threadedComment ref="B224" dT="2023-09-11T22:15:26.86" personId="{F2C253AE-3829-426F-8607-10F478AAC97A}" id="{BF13A08C-3A83-4A87-89AA-5677AE747C03}">
+    <text>This is the official USDA Plants code</text>
+  </threadedComment>
+  <threadedComment ref="B225" dT="2023-09-11T22:15:59.13" personId="{F2C253AE-3829-426F-8607-10F478AAC97A}" id="{C221EFA2-F912-4135-981C-E7AF98A329A9}">
+    <text>This is the official USDA Plants code</text>
+  </threadedComment>
+  <threadedComment ref="B372" dT="2023-09-11T22:13:34.20" personId="{F2C253AE-3829-426F-8607-10F478AAC97A}" id="{2F5931CB-DF6B-4F53-9005-53E77F3E2987}">
+    <text>Originally was "SPAM3", which was likely a mistake from dragging and copying the cell above at some point.</text>
+  </threadedComment>
+  <threadedComment ref="B373" dT="2023-09-11T22:13:45.25" personId="{F2C253AE-3829-426F-8607-10F478AAC97A}" id="{C6172F8C-64D1-435B-B6C6-C054FCF63812}">
+    <text>Originally was "SPAM4", which was likely a mistake from dragging and copying the cell above at some point.</text>
+  </threadedComment>
+  <threadedComment ref="B374" dT="2023-09-11T22:13:53.13" personId="{F2C253AE-3829-426F-8607-10F478AAC97A}" id="{7A5A69C5-6672-4327-A71A-D60D0159BC65}">
+    <text>Originally was "SPAM5", which was likely a mistake from dragging and copying the cell above at some point.</text>
+  </threadedComment>
+  <threadedComment ref="B391" dT="2023-09-11T22:17:46.96" personId="{F2C253AE-3829-426F-8607-10F478AAC97A}" id="{5B1E393E-188A-4FCD-87DD-803EDEB5A732}">
+    <text>This is the official USDA Plants code</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F397"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A380" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A392" sqref="A392:XFD392"/>
+      <pane ySplit="1" topLeftCell="A373" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D389" sqref="D389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6643,7 +6774,7 @@
       <c r="A195" t="s">
         <v>263</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B195" s="1" t="s">
         <v>260</v>
       </c>
       <c r="C195" t="s">
@@ -7223,8 +7354,8 @@
       <c r="A224" t="s">
         <v>314</v>
       </c>
-      <c r="B224" t="s">
-        <v>314</v>
+      <c r="B224" s="1" t="s">
+        <v>598</v>
       </c>
       <c r="C224" t="s">
         <v>315</v>
@@ -7243,8 +7374,8 @@
       <c r="A225" t="s">
         <v>316</v>
       </c>
-      <c r="B225" t="s">
-        <v>316</v>
+      <c r="B225" s="1" t="s">
+        <v>599</v>
       </c>
       <c r="C225" t="s">
         <v>317</v>
@@ -10563,8 +10694,8 @@
       <c r="A391" t="s">
         <v>584</v>
       </c>
-      <c r="B391" t="s">
-        <v>584</v>
+      <c r="B391" s="1" t="s">
+        <v>600</v>
       </c>
       <c r="C391" t="s">
         <v>585</v>
@@ -10703,5 +10834,6 @@
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final edits to edited-species8 & 9: deleted duplicate row of dependent, changed name to reflect subspecies specificity, as was changed manually earlier in code
</commit_message>
<xml_diff>
--- a/data/raw/01b_edited-species8_location-independent-final-fix.xlsx
+++ b/data/raw/01b_edited-species8_location-independent-final-fix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:40009_{8A6DA30E-687F-47E7-A24D-C265325037DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BD8F5B1-2932-45F6-B0B3-271EF40645C4}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:40009_{8A6DA30E-687F-47E7-A24D-C265325037DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53371BE5-1FC3-4F1C-A2FC-E8B39FEEA355}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2344" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2344" uniqueCount="602">
   <si>
     <t>CodeOriginal</t>
   </si>
@@ -1856,6 +1856,12 @@
   </si>
   <si>
     <t>S-PASM</t>
+  </si>
+  <si>
+    <t>Draba cuneifolia var. integrifolia</t>
+  </si>
+  <si>
+    <t>Eschscholzia californica ssp. Mexicana</t>
   </si>
 </sst>
 </file>
@@ -2351,9 +2357,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2807,8 +2816,8 @@
   <dimension ref="A1:F395"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C382" sqref="C382"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5428,8 +5437,8 @@
       <c r="B131" t="s">
         <v>257</v>
       </c>
-      <c r="C131" t="s">
-        <v>256</v>
+      <c r="C131" s="2" t="s">
+        <v>600</v>
       </c>
       <c r="D131" t="s">
         <v>3</v>
@@ -5989,7 +5998,7 @@
         <v>309</v>
       </c>
       <c r="C159" t="s">
-        <v>308</v>
+        <v>601</v>
       </c>
       <c r="D159" t="s">
         <v>3</v>

</xml_diff>